<commit_message>
Working on #6546; improved documentation Please merge
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Pinus/Observed.xlsx
+++ b/Tests/UnderReview/Pinus/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Tests\UnderReview\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C77FEB-D3B0-4E6B-8C74-EC61AD52C790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6826AF87-3219-43A7-8249-20D3B75E97EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17670" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="6" r:id="rId1"/>
@@ -148,42 +148,6 @@
   </si>
   <si>
     <t>Albaugh et al 1998, 2004</t>
-  </si>
-  <si>
-    <t>BeerwahPEE</t>
-  </si>
-  <si>
-    <t>BeerwahPCH</t>
-  </si>
-  <si>
-    <t>BeerwahF1</t>
-  </si>
-  <si>
-    <t>BeerwahF2</t>
-  </si>
-  <si>
-    <t>ToolaraPEE</t>
-  </si>
-  <si>
-    <t>ToolaraPCH</t>
-  </si>
-  <si>
-    <t>ToolaraF1</t>
-  </si>
-  <si>
-    <t>ToolaraF2</t>
-  </si>
-  <si>
-    <t>TuanPEE</t>
-  </si>
-  <si>
-    <t>TuanPCH</t>
-  </si>
-  <si>
-    <t>TuanF1</t>
-  </si>
-  <si>
-    <t>TuanF2</t>
   </si>
   <si>
     <t>Dieters and Brawner 2007</t>
@@ -375,28 +339,64 @@
     <t>Pinus.Cone.Live.NConc</t>
   </si>
   <si>
-    <t>HQP248MBRF1ContainerLargeMound</t>
-  </si>
-  <si>
-    <t>HQP251MBRF1MB6</t>
-  </si>
-  <si>
-    <t>HQP350GYMHighFWC</t>
-  </si>
-  <si>
     <t>FSA703A</t>
   </si>
   <si>
     <t>FSA704</t>
   </si>
   <si>
-    <t>HQP321GYMR1</t>
+    <t>stemspha</t>
   </si>
   <si>
-    <t>HQP321GYMBL2TWC</t>
+    <t>HQP321R1</t>
   </si>
   <si>
-    <t>stemspha</t>
+    <t>HQP321R2</t>
+  </si>
+  <si>
+    <t>HQP248</t>
+  </si>
+  <si>
+    <t>HQP251</t>
+  </si>
+  <si>
+    <t>HQP350</t>
+  </si>
+  <si>
+    <t>FPQBeerwah_PEE</t>
+  </si>
+  <si>
+    <t>FPQBeerwah_PCH</t>
+  </si>
+  <si>
+    <t>FPQBeerwah_F1</t>
+  </si>
+  <si>
+    <t>FPQBeerwah_F2</t>
+  </si>
+  <si>
+    <t>FPQToolara_PEE</t>
+  </si>
+  <si>
+    <t>FPQToolara_PCH</t>
+  </si>
+  <si>
+    <t>FPQToolara_F1</t>
+  </si>
+  <si>
+    <t>FPQToolara_F2</t>
+  </si>
+  <si>
+    <t>FPQTuan_PEE</t>
+  </si>
+  <si>
+    <t>FPQTuan_PCH</t>
+  </si>
+  <si>
+    <t>FPQTuan_F1</t>
+  </si>
+  <si>
+    <t>FPQTuan_F2</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1068,10 @@
   <dimension ref="A1:BT1505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="W371" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D1119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA497" sqref="AA378:AH497"/>
+      <selection pane="bottomRight" activeCell="A1136" sqref="A1136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -1124,46 +1124,46 @@
         <v>21</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="N1" s="29" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="O1" s="29" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="29" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="S1" s="29" t="s">
         <v>3</v>
@@ -1175,13 +1175,13 @@
         <v>25</v>
       </c>
       <c r="V1" s="29" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="X1" s="29" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="Y1" s="29" t="s">
         <v>2</v>
@@ -1190,55 +1190,55 @@
         <v>8</v>
       </c>
       <c r="AA1" s="29" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="AB1" s="29" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="AC1" s="29" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="AD1" s="29" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="AE1" s="44" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AF1" s="44" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="AG1" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH1" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI1" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ1" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="AH1" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI1" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ1" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="AK1" s="29" t="s">
-        <v>105</v>
-      </c>
       <c r="AL1" s="29" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="AM1" s="29" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="AN1" s="29" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="AO1" s="29" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="AP1" s="29" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="AQ1" s="29" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="AR1" s="29" t="s">
         <v>10</v>
@@ -1249,49 +1249,49 @@
       <c r="AT1" s="28"/>
       <c r="AU1" s="28"/>
       <c r="BF1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BR1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="BJ1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BK1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="BL1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BM1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="BN1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="BO1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BP1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="BQ1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="BR1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:72">
@@ -41132,7 +41132,7 @@
     </row>
     <row r="1050" spans="1:50">
       <c r="A1050" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1050" s="16">
         <v>26860</v>
@@ -41196,7 +41196,7 @@
     </row>
     <row r="1051" spans="1:50">
       <c r="A1051" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1051" s="5">
         <v>27590.484400000001</v>
@@ -41294,7 +41294,7 @@
     </row>
     <row r="1052" spans="1:50">
       <c r="A1052" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1052" s="5">
         <v>27955.726600000002</v>
@@ -41392,7 +41392,7 @@
     </row>
     <row r="1053" spans="1:50">
       <c r="A1053" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1053" s="5">
         <v>28320.968799999999</v>
@@ -41490,7 +41490,7 @@
     </row>
     <row r="1054" spans="1:50">
       <c r="A1054" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1054" s="5">
         <v>28686.210999999999</v>
@@ -41592,7 +41592,7 @@
     </row>
     <row r="1055" spans="1:50">
       <c r="A1055" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1055" s="5">
         <v>29047.800778000001</v>
@@ -41694,7 +41694,7 @@
     </row>
     <row r="1056" spans="1:50">
       <c r="A1056" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1056" s="5">
         <v>29051.4532</v>
@@ -41796,7 +41796,7 @@
     </row>
     <row r="1057" spans="1:50">
       <c r="A1057" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1057" s="5">
         <v>29416.695400000001</v>
@@ -41898,7 +41898,7 @@
     </row>
     <row r="1058" spans="1:50">
       <c r="A1058" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1058" s="5">
         <v>29781.937600000001</v>
@@ -42000,7 +42000,7 @@
     </row>
     <row r="1059" spans="1:50">
       <c r="A1059" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1059" s="5">
         <v>30147.179800000002</v>
@@ -42102,7 +42102,7 @@
     </row>
     <row r="1060" spans="1:50">
       <c r="A1060" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1060" s="5">
         <v>30508.769577999999</v>
@@ -42204,7 +42204,7 @@
     </row>
     <row r="1061" spans="1:50">
       <c r="A1061" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1061" s="5">
         <v>30512.421999999999</v>
@@ -42306,7 +42306,7 @@
     </row>
     <row r="1062" spans="1:50">
       <c r="A1062" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1062" s="5">
         <v>30877.664199999999</v>
@@ -42408,7 +42408,7 @@
     </row>
     <row r="1063" spans="1:50">
       <c r="A1063" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1063" s="5">
         <v>31242.9064</v>
@@ -42510,7 +42510,7 @@
     </row>
     <row r="1064" spans="1:50">
       <c r="A1064" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1064" s="5">
         <f>B1050+(C1064*365.2422)</f>
@@ -42573,7 +42573,7 @@
       <c r="AP1064" s="6"/>
       <c r="AQ1064" s="6"/>
       <c r="AR1064" s="35" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AS1064" s="36"/>
       <c r="AT1064" s="36"/>
@@ -42584,7 +42584,7 @@
     </row>
     <row r="1065" spans="1:50">
       <c r="A1065" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1065" s="5">
         <f>B1051+(C1065*365.2422)</f>
@@ -42647,7 +42647,7 @@
       <c r="AP1065" s="6"/>
       <c r="AQ1065" s="6"/>
       <c r="AR1065" s="35" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AS1065" s="36"/>
       <c r="AT1065" s="36"/>
@@ -42658,7 +42658,7 @@
     </row>
     <row r="1066" spans="1:50">
       <c r="A1066" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1066" s="5">
         <f>B1052+(C1066*365.2422)</f>
@@ -42721,7 +42721,7 @@
       <c r="AP1066" s="6"/>
       <c r="AQ1066" s="6"/>
       <c r="AR1066" s="35" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AS1066" s="36"/>
       <c r="AT1066" s="36"/>
@@ -42732,7 +42732,7 @@
     </row>
     <row r="1067" spans="1:50">
       <c r="A1067" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1067" s="16">
         <v>26860</v>
@@ -42794,7 +42794,7 @@
     </row>
     <row r="1068" spans="1:50">
       <c r="A1068" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1068" s="5">
         <v>27590.484400000001</v>
@@ -42864,7 +42864,7 @@
     </row>
     <row r="1069" spans="1:50">
       <c r="A1069" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1069" s="5">
         <v>27955.726600000002</v>
@@ -42934,7 +42934,7 @@
     </row>
     <row r="1070" spans="1:50">
       <c r="A1070" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1070" s="5">
         <v>28320.968799999999</v>
@@ -43004,7 +43004,7 @@
     </row>
     <row r="1071" spans="1:50">
       <c r="A1071" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1071" s="5">
         <v>28686.210999999999</v>
@@ -43075,7 +43075,7 @@
     </row>
     <row r="1072" spans="1:50">
       <c r="A1072" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1072" s="5">
         <v>29051.4532</v>
@@ -43146,7 +43146,7 @@
     </row>
     <row r="1073" spans="1:50">
       <c r="A1073" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1073" s="5">
         <v>29416.695400000001</v>
@@ -43217,7 +43217,7 @@
     </row>
     <row r="1074" spans="1:50">
       <c r="A1074" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1074" s="5">
         <v>29781.937600000001</v>
@@ -43288,7 +43288,7 @@
     </row>
     <row r="1075" spans="1:50">
       <c r="A1075" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1075" s="5">
         <v>30147.179800000002</v>
@@ -43359,7 +43359,7 @@
     </row>
     <row r="1076" spans="1:50">
       <c r="A1076" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1076" s="5">
         <v>30512.421999999999</v>
@@ -43430,7 +43430,7 @@
     </row>
     <row r="1077" spans="1:50">
       <c r="A1077" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1077" s="5">
         <v>30877.664199999999</v>
@@ -43501,7 +43501,7 @@
     </row>
     <row r="1078" spans="1:50">
       <c r="A1078" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1078" s="5">
         <v>31242.9064</v>
@@ -43600,7 +43600,7 @@
     </row>
     <row r="1079" spans="1:50">
       <c r="A1079" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1079" s="5">
         <f>B1067+(C1079*365.2422)</f>
@@ -43658,7 +43658,7 @@
       <c r="AP1079" s="6"/>
       <c r="AQ1079" s="6"/>
       <c r="AR1079" s="35" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AS1079" s="36"/>
       <c r="AT1079" s="36"/>
@@ -45849,7 +45849,7 @@
     </row>
     <row r="1136" spans="1:44">
       <c r="A1136" s="3" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="B1136" s="5">
         <v>35581.421999999999</v>
@@ -45865,12 +45865,12 @@
         <v>13.2</v>
       </c>
       <c r="AR1136" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1137" spans="1:44">
       <c r="A1137" s="3" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="B1137" s="5">
         <v>35581.421999999999</v>
@@ -45886,12 +45886,12 @@
         <v>17.100000000000001</v>
       </c>
       <c r="AR1137" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1138" spans="1:44">
       <c r="A1138" s="3" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="B1138" s="5">
         <v>35581.421999999999</v>
@@ -45907,12 +45907,12 @@
         <v>20</v>
       </c>
       <c r="AR1138" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1139" spans="1:44">
       <c r="A1139" s="3" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="B1139" s="5">
         <v>35581.421999999999</v>
@@ -45928,12 +45928,12 @@
         <v>18.899999999999999</v>
       </c>
       <c r="AR1139" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1140" spans="1:44">
       <c r="A1140" s="3" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="B1140" s="5">
         <v>35534.421999999999</v>
@@ -45949,12 +45949,12 @@
         <v>11.3</v>
       </c>
       <c r="AR1140" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1141" spans="1:44">
       <c r="A1141" s="3" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="B1141" s="5">
         <v>35534.421999999999</v>
@@ -45970,12 +45970,12 @@
         <v>18.8</v>
       </c>
       <c r="AR1141" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1142" spans="1:44">
       <c r="A1142" s="3" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="B1142" s="5">
         <v>35534.421999999999</v>
@@ -45991,12 +45991,12 @@
         <v>16.899999999999999</v>
       </c>
       <c r="AR1142" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1143" spans="1:44">
       <c r="A1143" s="3" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="B1143" s="5">
         <v>35534.421999999999</v>
@@ -46012,12 +46012,12 @@
         <v>16.3</v>
       </c>
       <c r="AR1143" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1144" spans="1:44">
       <c r="A1144" s="3" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="B1144" s="5">
         <v>35550.421999999999</v>
@@ -46033,12 +46033,12 @@
         <v>10.6</v>
       </c>
       <c r="AR1144" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1145" spans="1:44">
       <c r="A1145" s="3" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B1145" s="5">
         <v>35550.421999999999</v>
@@ -46054,12 +46054,12 @@
         <v>14.2</v>
       </c>
       <c r="AR1145" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1146" spans="1:44">
       <c r="A1146" s="3" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B1146" s="5">
         <v>35550.421999999999</v>
@@ -46075,12 +46075,12 @@
         <v>14.6</v>
       </c>
       <c r="AR1146" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1147" spans="1:44">
       <c r="A1147" s="3" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="B1147" s="5">
         <v>35550.421999999999</v>
@@ -46096,12 +46096,12 @@
         <v>13.5</v>
       </c>
       <c r="AR1147" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1148" spans="1:44">
       <c r="A1148" s="3" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="B1148" s="5">
         <v>37407.633000000002</v>
@@ -46128,12 +46128,12 @@
         <v>18.600000000000001</v>
       </c>
       <c r="AR1148" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1149" spans="1:44">
       <c r="A1149" s="3" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="B1149" s="5">
         <v>37407.633000000002</v>
@@ -46160,12 +46160,12 @@
         <v>22.7</v>
       </c>
       <c r="AR1149" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1150" spans="1:44">
       <c r="A1150" s="3" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="B1150" s="5">
         <v>37407.633000000002</v>
@@ -46192,12 +46192,12 @@
         <v>25.4</v>
       </c>
       <c r="AR1150" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1151" spans="1:44">
       <c r="A1151" s="3" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="B1151" s="5">
         <v>37407.633000000002</v>
@@ -46224,12 +46224,12 @@
         <v>25.1</v>
       </c>
       <c r="AR1151" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1152" spans="1:44">
       <c r="A1152" s="3" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="B1152" s="5">
         <v>37360.633000000002</v>
@@ -46256,12 +46256,12 @@
         <v>16.8</v>
       </c>
       <c r="AR1152" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1153" spans="1:44">
       <c r="A1153" s="3" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="B1153" s="5">
         <v>37360.633000000002</v>
@@ -46288,12 +46288,12 @@
         <v>24.9</v>
       </c>
       <c r="AR1153" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1154" spans="1:44">
       <c r="A1154" s="3" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="B1154" s="5">
         <v>37360.633000000002</v>
@@ -46320,12 +46320,12 @@
         <v>22</v>
       </c>
       <c r="AR1154" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1155" spans="1:44">
       <c r="A1155" s="3" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="B1155" s="5">
         <v>37360.633000000002</v>
@@ -46352,12 +46352,12 @@
         <v>22.1</v>
       </c>
       <c r="AR1155" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1156" spans="1:44">
       <c r="A1156" s="3" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="B1156" s="5">
         <v>37376.633000000002</v>
@@ -46384,12 +46384,12 @@
         <v>14.1</v>
       </c>
       <c r="AR1156" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1157" spans="1:44">
       <c r="A1157" s="3" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B1157" s="5">
         <v>37376.633000000002</v>
@@ -46416,12 +46416,12 @@
         <v>19.2</v>
       </c>
       <c r="AR1157" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1158" spans="1:44">
       <c r="A1158" s="3" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B1158" s="5">
         <v>37376.633000000002</v>
@@ -46448,12 +46448,12 @@
         <v>18.8</v>
       </c>
       <c r="AR1158" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1159" spans="1:44">
       <c r="A1159" s="3" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="B1159" s="5">
         <v>37376.633000000002</v>
@@ -46480,12 +46480,12 @@
         <v>17.7</v>
       </c>
       <c r="AR1159" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1160" spans="1:44">
       <c r="A1160" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1160" s="5">
         <v>36022.211000000003</v>
@@ -46502,7 +46502,7 @@
     </row>
     <row r="1161" spans="1:44">
       <c r="A1161" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1161" s="5">
         <v>36752.695400000004</v>
@@ -46531,7 +46531,7 @@
     </row>
     <row r="1162" spans="1:44">
       <c r="A1162" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1162" s="5">
         <v>37117.937600000005</v>
@@ -46560,7 +46560,7 @@
     </row>
     <row r="1163" spans="1:44">
       <c r="A1163" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1163" s="5">
         <v>37483.179800000005</v>
@@ -46589,7 +46589,7 @@
     </row>
     <row r="1164" spans="1:44">
       <c r="A1164" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1164" s="5">
         <v>37848.422000000006</v>
@@ -46618,7 +46618,7 @@
     </row>
     <row r="1165" spans="1:44">
       <c r="A1165" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1165" s="5">
         <v>38578.9064</v>
@@ -46647,7 +46647,7 @@
     </row>
     <row r="1166" spans="1:44">
       <c r="A1166" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1166" s="5">
         <v>38944.1486</v>
@@ -46676,7 +46676,7 @@
     </row>
     <row r="1167" spans="1:44">
       <c r="A1167" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1167" s="5">
         <v>39309.390800000001</v>
@@ -46705,7 +46705,7 @@
     </row>
     <row r="1168" spans="1:44">
       <c r="A1168" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1168" s="5">
         <v>39674.633000000002</v>
@@ -46734,7 +46734,7 @@
     </row>
     <row r="1169" spans="1:72">
       <c r="A1169" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1169" s="5">
         <v>22812</v>
@@ -46751,7 +46751,7 @@
     </row>
     <row r="1170" spans="1:72">
       <c r="A1170" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1170" s="5">
         <v>29021.117399999999</v>
@@ -46778,7 +46778,7 @@
     </row>
     <row r="1171" spans="1:72">
       <c r="A1171" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1171" s="5">
         <v>29386.3596</v>
@@ -46805,7 +46805,7 @@
     </row>
     <row r="1172" spans="1:72">
       <c r="A1172" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1172" s="5">
         <v>29751.6018</v>
@@ -46832,7 +46832,7 @@
     </row>
     <row r="1173" spans="1:72">
       <c r="A1173" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1173" s="5">
         <v>30116.844000000001</v>
@@ -46859,7 +46859,7 @@
     </row>
     <row r="1174" spans="1:72">
       <c r="A1174" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1174" s="5">
         <v>30482.086200000002</v>
@@ -46886,7 +46886,7 @@
     </row>
     <row r="1175" spans="1:72">
       <c r="A1175" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1175" s="5">
         <v>30847.328399999999</v>
@@ -46913,7 +46913,7 @@
     </row>
     <row r="1176" spans="1:72">
       <c r="A1176" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1176" s="5">
         <v>31212.570599999999</v>
@@ -46940,7 +46940,7 @@
     </row>
     <row r="1177" spans="1:72">
       <c r="A1177" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1177" s="5">
         <v>31577.8128</v>
@@ -46967,7 +46967,7 @@
     </row>
     <row r="1178" spans="1:72">
       <c r="A1178" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1178" s="5">
         <v>31943.055</v>
@@ -47083,7 +47083,7 @@
     </row>
     <row r="1179" spans="1:72" ht="15">
       <c r="A1179" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1179" s="5">
         <v>32308.297200000001</v>
@@ -47108,7 +47108,7 @@
     </row>
     <row r="1180" spans="1:72" ht="15">
       <c r="A1180" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1180" s="5">
         <v>32673.539400000001</v>
@@ -47136,7 +47136,7 @@
     </row>
     <row r="1181" spans="1:72">
       <c r="A1181" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1181" s="5">
         <v>33038.781600000002</v>
@@ -47164,7 +47164,7 @@
     </row>
     <row r="1182" spans="1:72">
       <c r="A1182" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1182" s="5">
         <v>33404.023800000003</v>
@@ -47251,7 +47251,7 @@
     </row>
     <row r="1183" spans="1:72">
       <c r="A1183" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1183" s="5">
         <v>33769.266000000003</v>
@@ -47278,7 +47278,7 @@
     </row>
     <row r="1184" spans="1:72">
       <c r="A1184" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1184" s="5">
         <v>34134.508199999997</v>
@@ -47305,7 +47305,7 @@
     </row>
     <row r="1185" spans="1:72">
       <c r="A1185" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1185" s="5">
         <v>34499.750400000004</v>
@@ -47332,7 +47332,7 @@
     </row>
     <row r="1186" spans="1:72">
       <c r="A1186" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1186" s="5">
         <v>34864.992599999998</v>
@@ -47359,7 +47359,7 @@
     </row>
     <row r="1187" spans="1:72">
       <c r="A1187" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1187" s="5">
         <v>35230.234799999998</v>
@@ -47446,7 +47446,7 @@
     </row>
     <row r="1188" spans="1:72">
       <c r="A1188" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1188" s="5">
         <v>22812</v>
@@ -47464,7 +47464,7 @@
     </row>
     <row r="1189" spans="1:72">
       <c r="A1189" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1189" s="5">
         <v>29021.117399999999</v>
@@ -47491,7 +47491,7 @@
     </row>
     <row r="1190" spans="1:72">
       <c r="A1190" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1190" s="5">
         <v>29386.3596</v>
@@ -47518,7 +47518,7 @@
     </row>
     <row r="1191" spans="1:72">
       <c r="A1191" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1191" s="5">
         <v>29751.6018</v>
@@ -47545,7 +47545,7 @@
     </row>
     <row r="1192" spans="1:72">
       <c r="A1192" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1192" s="5">
         <v>30116.844000000001</v>
@@ -47572,7 +47572,7 @@
     </row>
     <row r="1193" spans="1:72">
       <c r="A1193" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1193" s="5">
         <v>30482.086200000002</v>
@@ -47599,7 +47599,7 @@
     </row>
     <row r="1194" spans="1:72">
       <c r="A1194" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1194" s="5">
         <v>30847.328399999999</v>
@@ -47626,7 +47626,7 @@
     </row>
     <row r="1195" spans="1:72">
       <c r="A1195" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1195" s="5">
         <v>31212.570599999999</v>
@@ -47653,7 +47653,7 @@
     </row>
     <row r="1196" spans="1:72">
       <c r="A1196" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1196" s="5">
         <v>31577.8128</v>
@@ -47680,7 +47680,7 @@
     </row>
     <row r="1197" spans="1:72" ht="15">
       <c r="A1197" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1197" s="5">
         <v>31943.055</v>
@@ -47796,7 +47796,7 @@
     </row>
     <row r="1198" spans="1:72">
       <c r="A1198" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1198" s="5">
         <v>32308.297200000001</v>
@@ -47820,7 +47820,7 @@
     </row>
     <row r="1199" spans="1:72">
       <c r="A1199" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1199" s="5">
         <v>32673.539400000001</v>
@@ -47847,7 +47847,7 @@
     </row>
     <row r="1200" spans="1:72">
       <c r="A1200" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1200" s="5">
         <v>33038.781600000002</v>
@@ -47874,7 +47874,7 @@
     </row>
     <row r="1201" spans="1:72">
       <c r="A1201" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1201" s="5">
         <v>33404.023800000003</v>
@@ -47961,7 +47961,7 @@
     </row>
     <row r="1202" spans="1:72">
       <c r="A1202" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1202" s="5">
         <v>33769.266000000003</v>
@@ -47988,7 +47988,7 @@
     </row>
     <row r="1203" spans="1:72">
       <c r="A1203" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1203" s="5">
         <v>34134.508199999997</v>
@@ -48015,7 +48015,7 @@
     </row>
     <row r="1204" spans="1:72">
       <c r="A1204" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1204" s="5">
         <v>34499.750400000004</v>
@@ -48042,7 +48042,7 @@
     </row>
     <row r="1205" spans="1:72">
       <c r="A1205" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1205" s="5">
         <v>34864.992599999998</v>
@@ -48069,7 +48069,7 @@
     </row>
     <row r="1206" spans="1:72">
       <c r="A1206" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1206" s="5">
         <v>35230.234799999998</v>
@@ -48156,7 +48156,7 @@
     </row>
     <row r="1207" spans="1:72" s="20" customFormat="1">
       <c r="A1207" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1207" s="5">
         <v>30331</v>
@@ -48173,7 +48173,7 @@
     </row>
     <row r="1208" spans="1:72" s="20" customFormat="1">
       <c r="A1208" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1208" s="5">
         <v>31792</v>
@@ -48211,7 +48211,7 @@
     </row>
     <row r="1209" spans="1:72" s="20" customFormat="1">
       <c r="A1209" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1209" s="5">
         <v>32157.242200000001</v>
@@ -48246,7 +48246,7 @@
     </row>
     <row r="1210" spans="1:72" s="20" customFormat="1">
       <c r="A1210" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1210" s="5">
         <v>32522.484400000001</v>
@@ -48284,7 +48284,7 @@
     </row>
     <row r="1211" spans="1:72" s="20" customFormat="1">
       <c r="A1211" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1211" s="5">
         <v>32887.726600000002</v>
@@ -48319,7 +48319,7 @@
     </row>
     <row r="1212" spans="1:72" s="20" customFormat="1">
       <c r="A1212" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1212" s="5">
         <v>33618.211000000003</v>
@@ -48357,7 +48357,7 @@
     </row>
     <row r="1213" spans="1:72" s="20" customFormat="1">
       <c r="A1213" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1213" s="5">
         <v>33983.453200000004</v>
@@ -48395,7 +48395,7 @@
     </row>
     <row r="1214" spans="1:72" s="20" customFormat="1">
       <c r="A1214" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1214" s="5">
         <v>34348.695400000004</v>
@@ -48433,7 +48433,7 @@
     </row>
     <row r="1215" spans="1:72" s="20" customFormat="1">
       <c r="A1215" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1215" s="5">
         <v>35079.179800000005</v>
@@ -48471,7 +48471,7 @@
     </row>
     <row r="1216" spans="1:72" s="20" customFormat="1">
       <c r="A1216" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1216" s="5">
         <v>35444.422000000006</v>
@@ -48509,7 +48509,7 @@
     </row>
     <row r="1217" spans="1:30" s="20" customFormat="1">
       <c r="A1217" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1217" s="5">
         <v>35809.664200000007</v>
@@ -48547,7 +48547,7 @@
     </row>
     <row r="1218" spans="1:30" s="20" customFormat="1">
       <c r="A1218" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1218" s="5">
         <v>36174.906400000007</v>
@@ -48585,7 +48585,7 @@
     </row>
     <row r="1219" spans="1:30" s="20" customFormat="1">
       <c r="A1219" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1219" s="5">
         <v>36905.390800000008</v>
@@ -48623,7 +48623,7 @@
     </row>
     <row r="1220" spans="1:30" s="20" customFormat="1">
       <c r="A1220" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1220" s="5">
         <v>38366.359600000011</v>
@@ -48661,7 +48661,7 @@
     </row>
     <row r="1221" spans="1:30" s="20" customFormat="1">
       <c r="A1221" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1221" s="5">
         <v>39462.086200000012</v>
@@ -48699,7 +48699,7 @@
     </row>
     <row r="1222" spans="1:30" s="20" customFormat="1">
       <c r="A1222" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1222" s="5">
         <v>30331</v>
@@ -48716,7 +48716,7 @@
     </row>
     <row r="1223" spans="1:30" s="20" customFormat="1">
       <c r="A1223" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1223" s="5">
         <v>31792</v>
@@ -48754,7 +48754,7 @@
     </row>
     <row r="1224" spans="1:30" s="20" customFormat="1">
       <c r="A1224" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1224" s="5">
         <v>32157.242200000001</v>
@@ -48789,7 +48789,7 @@
     </row>
     <row r="1225" spans="1:30" s="20" customFormat="1">
       <c r="A1225" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1225" s="5">
         <v>32522.484400000001</v>
@@ -48827,7 +48827,7 @@
     </row>
     <row r="1226" spans="1:30" s="20" customFormat="1">
       <c r="A1226" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1226" s="5">
         <v>32887.726600000002</v>
@@ -48862,7 +48862,7 @@
     </row>
     <row r="1227" spans="1:30" s="20" customFormat="1">
       <c r="A1227" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1227" s="5">
         <v>33618.211000000003</v>
@@ -48900,7 +48900,7 @@
     </row>
     <row r="1228" spans="1:30" s="20" customFormat="1">
       <c r="A1228" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1228" s="5">
         <v>33983.453200000004</v>
@@ -48938,7 +48938,7 @@
     </row>
     <row r="1229" spans="1:30" s="20" customFormat="1">
       <c r="A1229" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1229" s="5">
         <v>34348.695400000004</v>
@@ -48976,7 +48976,7 @@
     </row>
     <row r="1230" spans="1:30" s="20" customFormat="1">
       <c r="A1230" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1230" s="5">
         <v>35079.179800000005</v>
@@ -49014,7 +49014,7 @@
     </row>
     <row r="1231" spans="1:30" s="20" customFormat="1">
       <c r="A1231" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1231" s="5">
         <v>35444.422000000006</v>
@@ -49052,7 +49052,7 @@
     </row>
     <row r="1232" spans="1:30" s="20" customFormat="1">
       <c r="A1232" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1232" s="5">
         <v>35809.664200000007</v>
@@ -49090,7 +49090,7 @@
     </row>
     <row r="1233" spans="1:30" s="20" customFormat="1">
       <c r="A1233" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1233" s="5">
         <v>36174.906400000007</v>
@@ -49128,7 +49128,7 @@
     </row>
     <row r="1234" spans="1:30" s="20" customFormat="1">
       <c r="A1234" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1234" s="5">
         <v>36905.390800000008</v>
@@ -49166,7 +49166,7 @@
     </row>
     <row r="1235" spans="1:30" s="20" customFormat="1">
       <c r="A1235" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1235" s="5">
         <v>38366.359600000011</v>
@@ -49204,7 +49204,7 @@
     </row>
     <row r="1236" spans="1:30" s="20" customFormat="1">
       <c r="A1236" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1236" s="5">
         <v>39462.086200000012</v>
@@ -49242,7 +49242,7 @@
     </row>
     <row r="1237" spans="1:30" s="20" customFormat="1">
       <c r="A1237" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1237" s="5">
         <v>30331</v>
@@ -49259,7 +49259,7 @@
     </row>
     <row r="1238" spans="1:30" s="20" customFormat="1">
       <c r="A1238" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1238" s="5">
         <v>31792</v>
@@ -49297,7 +49297,7 @@
     </row>
     <row r="1239" spans="1:30" s="20" customFormat="1">
       <c r="A1239" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1239" s="5">
         <v>32157.242200000001</v>
@@ -49332,7 +49332,7 @@
     </row>
     <row r="1240" spans="1:30" s="20" customFormat="1">
       <c r="A1240" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1240" s="5">
         <v>32522.484400000001</v>
@@ -49370,7 +49370,7 @@
     </row>
     <row r="1241" spans="1:30" s="20" customFormat="1">
       <c r="A1241" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1241" s="5">
         <v>32887.726600000002</v>
@@ -49405,7 +49405,7 @@
     </row>
     <row r="1242" spans="1:30" s="20" customFormat="1">
       <c r="A1242" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1242" s="5">
         <v>33618.211000000003</v>
@@ -49443,7 +49443,7 @@
     </row>
     <row r="1243" spans="1:30" s="20" customFormat="1">
       <c r="A1243" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1243" s="5">
         <v>33983.453200000004</v>
@@ -49481,7 +49481,7 @@
     </row>
     <row r="1244" spans="1:30" s="20" customFormat="1">
       <c r="A1244" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1244" s="5">
         <v>34348.695400000004</v>
@@ -49519,7 +49519,7 @@
     </row>
     <row r="1245" spans="1:30" s="20" customFormat="1">
       <c r="A1245" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1245" s="5">
         <v>35079.179800000005</v>
@@ -49557,7 +49557,7 @@
     </row>
     <row r="1246" spans="1:30" s="20" customFormat="1">
       <c r="A1246" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1246" s="5">
         <v>35444.422000000006</v>
@@ -49595,7 +49595,7 @@
     </row>
     <row r="1247" spans="1:30" s="20" customFormat="1">
       <c r="A1247" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1247" s="5">
         <v>35809.664200000007</v>
@@ -49633,7 +49633,7 @@
     </row>
     <row r="1248" spans="1:30" s="20" customFormat="1">
       <c r="A1248" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1248" s="5">
         <v>36174.906400000007</v>
@@ -49671,7 +49671,7 @@
     </row>
     <row r="1249" spans="1:30" s="20" customFormat="1">
       <c r="A1249" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1249" s="5">
         <v>36905.390800000008</v>
@@ -49709,7 +49709,7 @@
     </row>
     <row r="1250" spans="1:30" s="20" customFormat="1">
       <c r="A1250" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1250" s="5">
         <v>38366.359600000011</v>
@@ -49747,7 +49747,7 @@
     </row>
     <row r="1251" spans="1:30" s="20" customFormat="1">
       <c r="A1251" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1251" s="5">
         <v>39462.086200000012</v>
@@ -49785,7 +49785,7 @@
     </row>
     <row r="1252" spans="1:30" s="20" customFormat="1">
       <c r="A1252" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1252" s="5">
         <v>30331</v>
@@ -49802,7 +49802,7 @@
     </row>
     <row r="1253" spans="1:30" s="20" customFormat="1">
       <c r="A1253" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1253" s="5">
         <v>31792</v>
@@ -49840,7 +49840,7 @@
     </row>
     <row r="1254" spans="1:30" s="20" customFormat="1">
       <c r="A1254" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1254" s="5">
         <v>32157.242200000001</v>
@@ -49875,7 +49875,7 @@
     </row>
     <row r="1255" spans="1:30" s="20" customFormat="1">
       <c r="A1255" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1255" s="5">
         <v>32522.484400000001</v>
@@ -49913,7 +49913,7 @@
     </row>
     <row r="1256" spans="1:30" s="20" customFormat="1">
       <c r="A1256" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1256" s="5">
         <v>32887.726600000002</v>
@@ -49948,7 +49948,7 @@
     </row>
     <row r="1257" spans="1:30" s="20" customFormat="1">
       <c r="A1257" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1257" s="5">
         <v>33618.211000000003</v>
@@ -49986,7 +49986,7 @@
     </row>
     <row r="1258" spans="1:30" s="20" customFormat="1">
       <c r="A1258" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1258" s="5">
         <v>33983.453200000004</v>
@@ -50024,7 +50024,7 @@
     </row>
     <row r="1259" spans="1:30" s="20" customFormat="1">
       <c r="A1259" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1259" s="5">
         <v>34348.695400000004</v>
@@ -50062,7 +50062,7 @@
     </row>
     <row r="1260" spans="1:30" s="20" customFormat="1">
       <c r="A1260" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1260" s="5">
         <v>35079.179800000005</v>
@@ -50100,7 +50100,7 @@
     </row>
     <row r="1261" spans="1:30" s="20" customFormat="1">
       <c r="A1261" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1261" s="5">
         <v>35444.422000000006</v>
@@ -50138,7 +50138,7 @@
     </row>
     <row r="1262" spans="1:30" s="20" customFormat="1">
       <c r="A1262" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1262" s="5">
         <v>35809.664200000007</v>
@@ -50176,7 +50176,7 @@
     </row>
     <row r="1263" spans="1:30" s="20" customFormat="1">
       <c r="A1263" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1263" s="5">
         <v>36174.906400000007</v>
@@ -50214,7 +50214,7 @@
     </row>
     <row r="1264" spans="1:30" s="20" customFormat="1">
       <c r="A1264" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1264" s="5">
         <v>36905.390800000008</v>
@@ -50252,7 +50252,7 @@
     </row>
     <row r="1265" spans="1:30" s="20" customFormat="1">
       <c r="A1265" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1265" s="5">
         <v>38366.359600000011</v>
@@ -50290,7 +50290,7 @@
     </row>
     <row r="1266" spans="1:30" s="20" customFormat="1">
       <c r="A1266" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1266" s="5">
         <v>39462.086200000012</v>
@@ -50328,7 +50328,7 @@
     </row>
     <row r="1267" spans="1:30" s="20" customFormat="1">
       <c r="A1267" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1267" s="5">
         <v>30331</v>
@@ -50345,7 +50345,7 @@
     </row>
     <row r="1268" spans="1:30" s="20" customFormat="1">
       <c r="A1268" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1268" s="5">
         <v>31792</v>
@@ -50383,7 +50383,7 @@
     </row>
     <row r="1269" spans="1:30" s="20" customFormat="1">
       <c r="A1269" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1269" s="5">
         <v>32157.242200000001</v>
@@ -50418,7 +50418,7 @@
     </row>
     <row r="1270" spans="1:30" s="20" customFormat="1">
       <c r="A1270" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1270" s="5">
         <v>32522.484400000001</v>
@@ -50456,7 +50456,7 @@
     </row>
     <row r="1271" spans="1:30" s="20" customFormat="1">
       <c r="A1271" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1271" s="5">
         <v>32887.726600000002</v>
@@ -50491,7 +50491,7 @@
     </row>
     <row r="1272" spans="1:30" s="20" customFormat="1">
       <c r="A1272" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1272" s="5">
         <v>33618.211000000003</v>
@@ -50526,7 +50526,7 @@
     </row>
     <row r="1273" spans="1:30" s="20" customFormat="1">
       <c r="A1273" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1273" s="5">
         <v>33983.453200000004</v>
@@ -50561,7 +50561,7 @@
     </row>
     <row r="1274" spans="1:30" s="20" customFormat="1">
       <c r="A1274" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1274" s="5">
         <v>34348.695400000004</v>
@@ -50599,7 +50599,7 @@
     </row>
     <row r="1275" spans="1:30" s="20" customFormat="1">
       <c r="A1275" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1275" s="5">
         <v>35079.179800000005</v>
@@ -50634,7 +50634,7 @@
     </row>
     <row r="1276" spans="1:30" s="20" customFormat="1">
       <c r="A1276" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1276" s="5">
         <v>35444.422000000006</v>
@@ -50672,7 +50672,7 @@
     </row>
     <row r="1277" spans="1:30" s="20" customFormat="1">
       <c r="A1277" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1277" s="5">
         <v>35809.664200000007</v>
@@ -50710,7 +50710,7 @@
     </row>
     <row r="1278" spans="1:30" s="20" customFormat="1">
       <c r="A1278" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1278" s="5">
         <v>36174.906400000007</v>
@@ -50748,7 +50748,7 @@
     </row>
     <row r="1279" spans="1:30" s="20" customFormat="1">
       <c r="A1279" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1279" s="5">
         <v>36905.390800000008</v>
@@ -50786,7 +50786,7 @@
     </row>
     <row r="1280" spans="1:30" s="20" customFormat="1">
       <c r="A1280" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1280" s="5">
         <v>38366.359600000011</v>
@@ -50824,7 +50824,7 @@
     </row>
     <row r="1281" spans="1:30" s="20" customFormat="1">
       <c r="A1281" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1281" s="5">
         <v>39462.086200000012</v>
@@ -50862,7 +50862,7 @@
     </row>
     <row r="1282" spans="1:30" s="20" customFormat="1">
       <c r="A1282" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1282" s="5">
         <v>30331</v>
@@ -50879,7 +50879,7 @@
     </row>
     <row r="1283" spans="1:30" s="20" customFormat="1">
       <c r="A1283" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1283" s="5">
         <v>31792</v>
@@ -50917,7 +50917,7 @@
     </row>
     <row r="1284" spans="1:30" s="20" customFormat="1">
       <c r="A1284" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1284" s="5">
         <v>32157.242200000001</v>
@@ -50952,7 +50952,7 @@
     </row>
     <row r="1285" spans="1:30" s="20" customFormat="1">
       <c r="A1285" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1285" s="5">
         <v>32522.484400000001</v>
@@ -50990,7 +50990,7 @@
     </row>
     <row r="1286" spans="1:30" s="20" customFormat="1">
       <c r="A1286" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1286" s="5">
         <v>32887.726600000002</v>
@@ -51025,7 +51025,7 @@
     </row>
     <row r="1287" spans="1:30" s="20" customFormat="1">
       <c r="A1287" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1287" s="5">
         <v>33618.211000000003</v>
@@ -51060,7 +51060,7 @@
     </row>
     <row r="1288" spans="1:30" s="20" customFormat="1">
       <c r="A1288" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1288" s="5">
         <v>33983.453200000004</v>
@@ -51095,7 +51095,7 @@
     </row>
     <row r="1289" spans="1:30" s="20" customFormat="1">
       <c r="A1289" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1289" s="5">
         <v>34348.695400000004</v>
@@ -51133,7 +51133,7 @@
     </row>
     <row r="1290" spans="1:30" s="20" customFormat="1">
       <c r="A1290" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1290" s="5">
         <v>35079.179800000005</v>
@@ -51168,7 +51168,7 @@
     </row>
     <row r="1291" spans="1:30" s="20" customFormat="1">
       <c r="A1291" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1291" s="5">
         <v>35444.422000000006</v>
@@ -51206,7 +51206,7 @@
     </row>
     <row r="1292" spans="1:30" s="20" customFormat="1">
       <c r="A1292" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1292" s="5">
         <v>35809.664200000007</v>
@@ -51244,7 +51244,7 @@
     </row>
     <row r="1293" spans="1:30" s="20" customFormat="1">
       <c r="A1293" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1293" s="5">
         <v>36174.906400000007</v>
@@ -51282,7 +51282,7 @@
     </row>
     <row r="1294" spans="1:30" s="20" customFormat="1">
       <c r="A1294" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1294" s="5">
         <v>36905.390800000008</v>
@@ -51320,7 +51320,7 @@
     </row>
     <row r="1295" spans="1:30" s="20" customFormat="1">
       <c r="A1295" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1295" s="5">
         <v>38366.359600000011</v>
@@ -51358,7 +51358,7 @@
     </row>
     <row r="1296" spans="1:30" s="20" customFormat="1">
       <c r="A1296" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1296" s="5">
         <v>39462.086200000012</v>
@@ -51396,7 +51396,7 @@
     </row>
     <row r="1297" spans="1:30" s="20" customFormat="1">
       <c r="A1297" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1297" s="5">
         <v>30331</v>
@@ -51413,7 +51413,7 @@
     </row>
     <row r="1298" spans="1:30" s="20" customFormat="1">
       <c r="A1298" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1298" s="5">
         <v>31792</v>
@@ -51451,7 +51451,7 @@
     </row>
     <row r="1299" spans="1:30" s="20" customFormat="1">
       <c r="A1299" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1299" s="5">
         <v>32157.242200000001</v>
@@ -51486,7 +51486,7 @@
     </row>
     <row r="1300" spans="1:30" s="20" customFormat="1">
       <c r="A1300" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1300" s="5">
         <v>32522.484400000001</v>
@@ -51524,7 +51524,7 @@
     </row>
     <row r="1301" spans="1:30" s="20" customFormat="1">
       <c r="A1301" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1301" s="5">
         <v>32887.726600000002</v>
@@ -51559,7 +51559,7 @@
     </row>
     <row r="1302" spans="1:30" s="20" customFormat="1">
       <c r="A1302" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1302" s="5">
         <v>33618.211000000003</v>
@@ -51594,7 +51594,7 @@
     </row>
     <row r="1303" spans="1:30" s="20" customFormat="1">
       <c r="A1303" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1303" s="5">
         <v>33983.453200000004</v>
@@ -51629,7 +51629,7 @@
     </row>
     <row r="1304" spans="1:30" s="20" customFormat="1">
       <c r="A1304" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1304" s="5">
         <v>34348.695400000004</v>
@@ -51667,7 +51667,7 @@
     </row>
     <row r="1305" spans="1:30" s="20" customFormat="1">
       <c r="A1305" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1305" s="5">
         <v>35079.179800000005</v>
@@ -51702,7 +51702,7 @@
     </row>
     <row r="1306" spans="1:30" s="20" customFormat="1">
       <c r="A1306" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1306" s="5">
         <v>35444.422000000006</v>
@@ -51740,7 +51740,7 @@
     </row>
     <row r="1307" spans="1:30" s="20" customFormat="1">
       <c r="A1307" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1307" s="5">
         <v>35809.664200000007</v>
@@ -51778,7 +51778,7 @@
     </row>
     <row r="1308" spans="1:30" s="20" customFormat="1">
       <c r="A1308" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1308" s="5">
         <v>36174.906400000007</v>
@@ -51816,7 +51816,7 @@
     </row>
     <row r="1309" spans="1:30" s="20" customFormat="1">
       <c r="A1309" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1309" s="5">
         <v>36905.390800000008</v>
@@ -51854,7 +51854,7 @@
     </row>
     <row r="1310" spans="1:30" s="20" customFormat="1">
       <c r="A1310" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1310" s="5">
         <v>38366.359600000011</v>
@@ -51892,7 +51892,7 @@
     </row>
     <row r="1311" spans="1:30" s="20" customFormat="1">
       <c r="A1311" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1311" s="5">
         <v>39462.086200000012</v>
@@ -51930,7 +51930,7 @@
     </row>
     <row r="1312" spans="1:30" s="20" customFormat="1">
       <c r="A1312" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1312" s="5">
         <v>30331</v>
@@ -51947,7 +51947,7 @@
     </row>
     <row r="1313" spans="1:30" s="20" customFormat="1">
       <c r="A1313" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1313" s="5">
         <v>31792</v>
@@ -51985,7 +51985,7 @@
     </row>
     <row r="1314" spans="1:30" s="20" customFormat="1">
       <c r="A1314" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1314" s="5">
         <v>32157.242200000001</v>
@@ -52020,7 +52020,7 @@
     </row>
     <row r="1315" spans="1:30" s="20" customFormat="1">
       <c r="A1315" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1315" s="5">
         <v>32522.484400000001</v>
@@ -52058,7 +52058,7 @@
     </row>
     <row r="1316" spans="1:30" s="20" customFormat="1">
       <c r="A1316" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1316" s="5">
         <v>32887.726600000002</v>
@@ -52093,7 +52093,7 @@
     </row>
     <row r="1317" spans="1:30" s="20" customFormat="1">
       <c r="A1317" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1317" s="5">
         <v>33618.211000000003</v>
@@ -52128,7 +52128,7 @@
     </row>
     <row r="1318" spans="1:30" s="20" customFormat="1">
       <c r="A1318" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1318" s="5">
         <v>33983.453200000004</v>
@@ -52163,7 +52163,7 @@
     </row>
     <row r="1319" spans="1:30" s="20" customFormat="1">
       <c r="A1319" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1319" s="5">
         <v>34348.695400000004</v>
@@ -52201,7 +52201,7 @@
     </row>
     <row r="1320" spans="1:30" s="20" customFormat="1">
       <c r="A1320" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1320" s="5">
         <v>35079.179800000005</v>
@@ -52236,7 +52236,7 @@
     </row>
     <row r="1321" spans="1:30" s="20" customFormat="1">
       <c r="A1321" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1321" s="5">
         <v>35444.422000000006</v>
@@ -52274,7 +52274,7 @@
     </row>
     <row r="1322" spans="1:30" s="20" customFormat="1">
       <c r="A1322" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1322" s="5">
         <v>35809.664200000007</v>
@@ -52312,7 +52312,7 @@
     </row>
     <row r="1323" spans="1:30" s="20" customFormat="1">
       <c r="A1323" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1323" s="5">
         <v>36174.906400000007</v>
@@ -52350,7 +52350,7 @@
     </row>
     <row r="1324" spans="1:30" s="20" customFormat="1">
       <c r="A1324" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1324" s="5">
         <v>36905.390800000008</v>
@@ -52388,7 +52388,7 @@
     </row>
     <row r="1325" spans="1:30" s="20" customFormat="1">
       <c r="A1325" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1325" s="5">
         <v>38366.359600000011</v>
@@ -52426,7 +52426,7 @@
     </row>
     <row r="1326" spans="1:30" s="20" customFormat="1">
       <c r="A1326" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1326" s="5">
         <v>39462.086200000012</v>
@@ -52464,7 +52464,7 @@
     </row>
     <row r="1327" spans="1:30" s="20" customFormat="1">
       <c r="A1327" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1327" s="5">
         <v>32523</v>
@@ -52482,7 +52482,7 @@
     </row>
     <row r="1328" spans="1:30" s="20" customFormat="1">
       <c r="A1328" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1328" s="5">
         <v>32888.242200000001</v>
@@ -52500,7 +52500,7 @@
     </row>
     <row r="1329" spans="1:21" s="20" customFormat="1">
       <c r="A1329" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1329" s="5">
         <v>33253.484400000001</v>
@@ -52518,7 +52518,7 @@
     </row>
     <row r="1330" spans="1:21" s="20" customFormat="1">
       <c r="A1330" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1330" s="5">
         <v>33618.726600000002</v>
@@ -52536,7 +52536,7 @@
     </row>
     <row r="1331" spans="1:21" s="20" customFormat="1">
       <c r="A1331" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1331" s="5">
         <v>33983.968800000002</v>
@@ -52554,7 +52554,7 @@
     </row>
     <row r="1332" spans="1:21" s="20" customFormat="1">
       <c r="A1332" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1332" s="5">
         <v>34349.211000000003</v>
@@ -52572,7 +52572,7 @@
     </row>
     <row r="1333" spans="1:21" s="20" customFormat="1">
       <c r="A1333" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1333" s="5">
         <v>34714.453200000004</v>
@@ -52590,7 +52590,7 @@
     </row>
     <row r="1334" spans="1:21" s="20" customFormat="1">
       <c r="A1334" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1334" s="5">
         <v>35079.695400000004</v>
@@ -52608,7 +52608,7 @@
     </row>
     <row r="1335" spans="1:21" s="20" customFormat="1">
       <c r="A1335" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1335" s="5">
         <v>35444.937600000005</v>
@@ -52626,7 +52626,7 @@
     </row>
     <row r="1336" spans="1:21" s="20" customFormat="1">
       <c r="A1336" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1336" s="5">
         <v>35810.179800000005</v>
@@ -52644,7 +52644,7 @@
     </row>
     <row r="1337" spans="1:21" s="20" customFormat="1">
       <c r="A1337" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1337" s="5">
         <v>36175.422000000006</v>
@@ -52662,7 +52662,7 @@
     </row>
     <row r="1338" spans="1:21" s="20" customFormat="1">
       <c r="A1338" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1338" s="5">
         <v>36540.664200000007</v>
@@ -52680,7 +52680,7 @@
     </row>
     <row r="1339" spans="1:21" s="20" customFormat="1">
       <c r="A1339" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1339" s="5">
         <v>36905.906400000007</v>
@@ -52698,7 +52698,7 @@
     </row>
     <row r="1340" spans="1:21" s="20" customFormat="1">
       <c r="A1340" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1340" s="5">
         <v>37271.148600000008</v>
@@ -52716,7 +52716,7 @@
     </row>
     <row r="1341" spans="1:21" s="20" customFormat="1">
       <c r="A1341" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1341" s="5">
         <v>32523</v>
@@ -52734,7 +52734,7 @@
     </row>
     <row r="1342" spans="1:21" s="20" customFormat="1">
       <c r="A1342" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1342" s="5">
         <v>32888.242200000001</v>
@@ -52752,7 +52752,7 @@
     </row>
     <row r="1343" spans="1:21" s="20" customFormat="1">
       <c r="A1343" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1343" s="5">
         <v>33253.484400000001</v>
@@ -52770,7 +52770,7 @@
     </row>
     <row r="1344" spans="1:21" s="20" customFormat="1">
       <c r="A1344" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1344" s="5">
         <v>33618.726600000002</v>
@@ -52788,7 +52788,7 @@
     </row>
     <row r="1345" spans="1:21" s="20" customFormat="1">
       <c r="A1345" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1345" s="5">
         <v>33983.968800000002</v>
@@ -52806,7 +52806,7 @@
     </row>
     <row r="1346" spans="1:21" s="20" customFormat="1">
       <c r="A1346" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1346" s="5">
         <v>34349.211000000003</v>
@@ -52824,7 +52824,7 @@
     </row>
     <row r="1347" spans="1:21" s="20" customFormat="1">
       <c r="A1347" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1347" s="5">
         <v>34714.453200000004</v>
@@ -52842,7 +52842,7 @@
     </row>
     <row r="1348" spans="1:21" s="20" customFormat="1">
       <c r="A1348" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1348" s="5">
         <v>35079.695400000004</v>
@@ -52860,7 +52860,7 @@
     </row>
     <row r="1349" spans="1:21" s="20" customFormat="1">
       <c r="A1349" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1349" s="5">
         <v>35444.937600000005</v>
@@ -52878,7 +52878,7 @@
     </row>
     <row r="1350" spans="1:21" s="20" customFormat="1">
       <c r="A1350" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1350" s="5">
         <v>35810.179800000005</v>
@@ -52896,7 +52896,7 @@
     </row>
     <row r="1351" spans="1:21" s="20" customFormat="1">
       <c r="A1351" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1351" s="5">
         <v>36175.422000000006</v>
@@ -52914,7 +52914,7 @@
     </row>
     <row r="1352" spans="1:21" s="20" customFormat="1">
       <c r="A1352" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1352" s="5">
         <v>36540.664200000007</v>
@@ -52932,7 +52932,7 @@
     </row>
     <row r="1353" spans="1:21" s="20" customFormat="1">
       <c r="A1353" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1353" s="5">
         <v>36905.906400000007</v>
@@ -52950,7 +52950,7 @@
     </row>
     <row r="1354" spans="1:21" s="20" customFormat="1">
       <c r="A1354" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1354" s="5">
         <v>37271.148600000008</v>
@@ -52968,7 +52968,7 @@
     </row>
     <row r="1355" spans="1:21" s="20" customFormat="1">
       <c r="A1355" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1355" s="5">
         <v>32523</v>
@@ -52986,7 +52986,7 @@
     </row>
     <row r="1356" spans="1:21" s="20" customFormat="1">
       <c r="A1356" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1356" s="5">
         <v>32888.242200000001</v>
@@ -53004,7 +53004,7 @@
     </row>
     <row r="1357" spans="1:21" s="20" customFormat="1">
       <c r="A1357" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1357" s="5">
         <v>33253.484400000001</v>
@@ -53022,7 +53022,7 @@
     </row>
     <row r="1358" spans="1:21" s="20" customFormat="1">
       <c r="A1358" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1358" s="5">
         <v>33618.726600000002</v>
@@ -53040,7 +53040,7 @@
     </row>
     <row r="1359" spans="1:21" s="20" customFormat="1">
       <c r="A1359" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1359" s="5">
         <v>33983.968800000002</v>
@@ -53058,7 +53058,7 @@
     </row>
     <row r="1360" spans="1:21" s="20" customFormat="1">
       <c r="A1360" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1360" s="5">
         <v>34349.211000000003</v>
@@ -53076,7 +53076,7 @@
     </row>
     <row r="1361" spans="1:21" s="20" customFormat="1">
       <c r="A1361" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1361" s="5">
         <v>34714.453200000004</v>
@@ -53094,7 +53094,7 @@
     </row>
     <row r="1362" spans="1:21" s="20" customFormat="1">
       <c r="A1362" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1362" s="5">
         <v>35079.695400000004</v>
@@ -53112,7 +53112,7 @@
     </row>
     <row r="1363" spans="1:21" s="20" customFormat="1">
       <c r="A1363" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1363" s="5">
         <v>35444.937600000005</v>
@@ -53130,7 +53130,7 @@
     </row>
     <row r="1364" spans="1:21" s="20" customFormat="1">
       <c r="A1364" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1364" s="5">
         <v>35810.179800000005</v>
@@ -53148,7 +53148,7 @@
     </row>
     <row r="1365" spans="1:21" s="20" customFormat="1">
       <c r="A1365" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1365" s="5">
         <v>36175.422000000006</v>
@@ -53166,7 +53166,7 @@
     </row>
     <row r="1366" spans="1:21" s="20" customFormat="1">
       <c r="A1366" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1366" s="5">
         <v>36540.664200000007</v>
@@ -53184,7 +53184,7 @@
     </row>
     <row r="1367" spans="1:21" s="20" customFormat="1">
       <c r="A1367" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1367" s="5">
         <v>36905.906400000007</v>
@@ -53202,7 +53202,7 @@
     </row>
     <row r="1368" spans="1:21" s="20" customFormat="1">
       <c r="A1368" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1368" s="5">
         <v>37271.148600000008</v>
@@ -53220,7 +53220,7 @@
     </row>
     <row r="1369" spans="1:21" s="20" customFormat="1">
       <c r="A1369" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1369" s="5">
         <v>32523</v>
@@ -53238,7 +53238,7 @@
     </row>
     <row r="1370" spans="1:21" s="20" customFormat="1">
       <c r="A1370" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1370" s="5">
         <v>32888.242200000001</v>
@@ -53256,7 +53256,7 @@
     </row>
     <row r="1371" spans="1:21" s="20" customFormat="1">
       <c r="A1371" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1371" s="5">
         <v>33253.484400000001</v>
@@ -53274,7 +53274,7 @@
     </row>
     <row r="1372" spans="1:21" s="20" customFormat="1">
       <c r="A1372" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1372" s="5">
         <v>33618.726600000002</v>
@@ -53292,7 +53292,7 @@
     </row>
     <row r="1373" spans="1:21" s="20" customFormat="1">
       <c r="A1373" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1373" s="5">
         <v>33983.968800000002</v>
@@ -53310,7 +53310,7 @@
     </row>
     <row r="1374" spans="1:21" s="20" customFormat="1">
       <c r="A1374" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1374" s="5">
         <v>34349.211000000003</v>
@@ -53328,7 +53328,7 @@
     </row>
     <row r="1375" spans="1:21" s="20" customFormat="1">
       <c r="A1375" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1375" s="5">
         <v>34714.453200000004</v>
@@ -53346,7 +53346,7 @@
     </row>
     <row r="1376" spans="1:21" s="20" customFormat="1">
       <c r="A1376" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1376" s="5">
         <v>35079.695400000004</v>
@@ -53364,7 +53364,7 @@
     </row>
     <row r="1377" spans="1:21" s="20" customFormat="1">
       <c r="A1377" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1377" s="5">
         <v>35444.937600000005</v>
@@ -53382,7 +53382,7 @@
     </row>
     <row r="1378" spans="1:21" s="20" customFormat="1">
       <c r="A1378" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1378" s="5">
         <v>35810.179800000005</v>
@@ -53400,7 +53400,7 @@
     </row>
     <row r="1379" spans="1:21" s="20" customFormat="1">
       <c r="A1379" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1379" s="5">
         <v>36175.422000000006</v>
@@ -53418,7 +53418,7 @@
     </row>
     <row r="1380" spans="1:21" s="20" customFormat="1">
       <c r="A1380" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1380" s="5">
         <v>36540.664200000007</v>
@@ -53436,7 +53436,7 @@
     </row>
     <row r="1381" spans="1:21" s="20" customFormat="1">
       <c r="A1381" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1381" s="5">
         <v>36905.906400000007</v>
@@ -53454,7 +53454,7 @@
     </row>
     <row r="1382" spans="1:21" s="20" customFormat="1">
       <c r="A1382" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B1382" s="5">
         <v>37271.148600000008</v>
@@ -53472,7 +53472,7 @@
     </row>
     <row r="1383" spans="1:21" s="20" customFormat="1">
       <c r="A1383" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1383" s="5">
         <v>32523</v>
@@ -53490,7 +53490,7 @@
     </row>
     <row r="1384" spans="1:21" s="20" customFormat="1">
       <c r="A1384" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1384" s="5">
         <v>32888.242200000001</v>
@@ -53508,7 +53508,7 @@
     </row>
     <row r="1385" spans="1:21" s="20" customFormat="1">
       <c r="A1385" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1385" s="5">
         <v>33253.484400000001</v>
@@ -53526,7 +53526,7 @@
     </row>
     <row r="1386" spans="1:21" s="20" customFormat="1">
       <c r="A1386" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1386" s="5">
         <v>33618.726600000002</v>
@@ -53544,7 +53544,7 @@
     </row>
     <row r="1387" spans="1:21" s="20" customFormat="1">
       <c r="A1387" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1387" s="5">
         <v>33983.968800000002</v>
@@ -53562,7 +53562,7 @@
     </row>
     <row r="1388" spans="1:21" s="20" customFormat="1">
       <c r="A1388" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1388" s="5">
         <v>34349.211000000003</v>
@@ -53580,7 +53580,7 @@
     </row>
     <row r="1389" spans="1:21" s="20" customFormat="1">
       <c r="A1389" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1389" s="5">
         <v>34714.453200000004</v>
@@ -53598,7 +53598,7 @@
     </row>
     <row r="1390" spans="1:21" s="20" customFormat="1">
       <c r="A1390" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1390" s="5">
         <v>35079.695400000004</v>
@@ -53616,7 +53616,7 @@
     </row>
     <row r="1391" spans="1:21" s="20" customFormat="1">
       <c r="A1391" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1391" s="5">
         <v>35444.937600000005</v>
@@ -53634,7 +53634,7 @@
     </row>
     <row r="1392" spans="1:21" s="20" customFormat="1">
       <c r="A1392" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1392" s="5">
         <v>35810.179800000005</v>
@@ -53652,7 +53652,7 @@
     </row>
     <row r="1393" spans="1:21" s="20" customFormat="1">
       <c r="A1393" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1393" s="5">
         <v>36175.422000000006</v>
@@ -53670,7 +53670,7 @@
     </row>
     <row r="1394" spans="1:21" s="20" customFormat="1">
       <c r="A1394" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1394" s="5">
         <v>36540.664200000007</v>
@@ -53688,7 +53688,7 @@
     </row>
     <row r="1395" spans="1:21" s="20" customFormat="1">
       <c r="A1395" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1395" s="5">
         <v>36905.906400000007</v>
@@ -53706,7 +53706,7 @@
     </row>
     <row r="1396" spans="1:21" s="20" customFormat="1">
       <c r="A1396" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B1396" s="5">
         <v>37271.148600000008</v>
@@ -53724,7 +53724,7 @@
     </row>
     <row r="1397" spans="1:21" s="20" customFormat="1">
       <c r="A1397" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1397" s="5">
         <v>32523</v>
@@ -53742,7 +53742,7 @@
     </row>
     <row r="1398" spans="1:21" s="20" customFormat="1">
       <c r="A1398" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1398" s="5">
         <v>32888.242200000001</v>
@@ -53760,7 +53760,7 @@
     </row>
     <row r="1399" spans="1:21" s="20" customFormat="1">
       <c r="A1399" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1399" s="5">
         <v>33253.484400000001</v>
@@ -53778,7 +53778,7 @@
     </row>
     <row r="1400" spans="1:21" s="20" customFormat="1">
       <c r="A1400" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1400" s="5">
         <v>33618.726600000002</v>
@@ -53796,7 +53796,7 @@
     </row>
     <row r="1401" spans="1:21" s="20" customFormat="1">
       <c r="A1401" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1401" s="5">
         <v>33983.968800000002</v>
@@ -53814,7 +53814,7 @@
     </row>
     <row r="1402" spans="1:21" s="20" customFormat="1">
       <c r="A1402" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1402" s="5">
         <v>34349.211000000003</v>
@@ -53832,7 +53832,7 @@
     </row>
     <row r="1403" spans="1:21" s="20" customFormat="1">
       <c r="A1403" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1403" s="5">
         <v>34714.453200000004</v>
@@ -53850,7 +53850,7 @@
     </row>
     <row r="1404" spans="1:21" s="20" customFormat="1">
       <c r="A1404" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1404" s="5">
         <v>35079.695400000004</v>
@@ -53868,7 +53868,7 @@
     </row>
     <row r="1405" spans="1:21" s="20" customFormat="1">
       <c r="A1405" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1405" s="5">
         <v>35444.937600000005</v>
@@ -53886,7 +53886,7 @@
     </row>
     <row r="1406" spans="1:21" s="20" customFormat="1">
       <c r="A1406" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1406" s="5">
         <v>35810.179800000005</v>
@@ -53904,7 +53904,7 @@
     </row>
     <row r="1407" spans="1:21" s="20" customFormat="1">
       <c r="A1407" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1407" s="5">
         <v>36175.422000000006</v>
@@ -53922,7 +53922,7 @@
     </row>
     <row r="1408" spans="1:21" s="20" customFormat="1">
       <c r="A1408" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1408" s="5">
         <v>36540.664200000007</v>
@@ -53940,7 +53940,7 @@
     </row>
     <row r="1409" spans="1:21" s="20" customFormat="1">
       <c r="A1409" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1409" s="5">
         <v>36905.906400000007</v>
@@ -53958,7 +53958,7 @@
     </row>
     <row r="1410" spans="1:21" s="20" customFormat="1">
       <c r="A1410" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B1410" s="5">
         <v>37271.148600000008</v>
@@ -53976,7 +53976,7 @@
     </row>
     <row r="1411" spans="1:21" s="20" customFormat="1">
       <c r="A1411" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1411" s="5">
         <v>32523</v>
@@ -53994,7 +53994,7 @@
     </row>
     <row r="1412" spans="1:21" s="20" customFormat="1">
       <c r="A1412" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1412" s="5">
         <v>32888.242200000001</v>
@@ -54012,7 +54012,7 @@
     </row>
     <row r="1413" spans="1:21" s="20" customFormat="1">
       <c r="A1413" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1413" s="5">
         <v>33253.484400000001</v>
@@ -54030,7 +54030,7 @@
     </row>
     <row r="1414" spans="1:21" s="20" customFormat="1">
       <c r="A1414" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1414" s="5">
         <v>33618.726600000002</v>
@@ -54048,7 +54048,7 @@
     </row>
     <row r="1415" spans="1:21" s="20" customFormat="1">
       <c r="A1415" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1415" s="5">
         <v>33983.968800000002</v>
@@ -54066,7 +54066,7 @@
     </row>
     <row r="1416" spans="1:21" s="20" customFormat="1">
       <c r="A1416" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1416" s="5">
         <v>34349.211000000003</v>
@@ -54084,7 +54084,7 @@
     </row>
     <row r="1417" spans="1:21" s="20" customFormat="1">
       <c r="A1417" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1417" s="5">
         <v>34714.453200000004</v>
@@ -54102,7 +54102,7 @@
     </row>
     <row r="1418" spans="1:21" s="20" customFormat="1">
       <c r="A1418" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1418" s="5">
         <v>35079.695400000004</v>
@@ -54120,7 +54120,7 @@
     </row>
     <row r="1419" spans="1:21" s="20" customFormat="1">
       <c r="A1419" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1419" s="5">
         <v>35444.937600000005</v>
@@ -54138,7 +54138,7 @@
     </row>
     <row r="1420" spans="1:21" s="20" customFormat="1">
       <c r="A1420" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1420" s="5">
         <v>35810.179800000005</v>
@@ -54156,7 +54156,7 @@
     </row>
     <row r="1421" spans="1:21" s="20" customFormat="1">
       <c r="A1421" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1421" s="5">
         <v>36175.422000000006</v>
@@ -54174,7 +54174,7 @@
     </row>
     <row r="1422" spans="1:21" s="20" customFormat="1">
       <c r="A1422" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1422" s="5">
         <v>36540.664200000007</v>
@@ -54192,7 +54192,7 @@
     </row>
     <row r="1423" spans="1:21" s="20" customFormat="1">
       <c r="A1423" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1423" s="5">
         <v>36905.906400000007</v>
@@ -54210,7 +54210,7 @@
     </row>
     <row r="1424" spans="1:21" s="20" customFormat="1">
       <c r="A1424" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B1424" s="5">
         <v>37271.148600000008</v>
@@ -54228,7 +54228,7 @@
     </row>
     <row r="1425" spans="1:21" s="20" customFormat="1">
       <c r="A1425" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1425" s="5">
         <v>32523</v>
@@ -54246,7 +54246,7 @@
     </row>
     <row r="1426" spans="1:21" s="20" customFormat="1">
       <c r="A1426" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1426" s="5">
         <v>32888.242200000001</v>
@@ -54264,7 +54264,7 @@
     </row>
     <row r="1427" spans="1:21" s="20" customFormat="1">
       <c r="A1427" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1427" s="5">
         <v>33253.484400000001</v>
@@ -54282,7 +54282,7 @@
     </row>
     <row r="1428" spans="1:21" s="20" customFormat="1">
       <c r="A1428" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1428" s="5">
         <v>33618.726600000002</v>
@@ -54300,7 +54300,7 @@
     </row>
     <row r="1429" spans="1:21" s="20" customFormat="1">
       <c r="A1429" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1429" s="5">
         <v>33983.968800000002</v>
@@ -54318,7 +54318,7 @@
     </row>
     <row r="1430" spans="1:21" s="20" customFormat="1">
       <c r="A1430" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1430" s="5">
         <v>34349.211000000003</v>
@@ -54336,7 +54336,7 @@
     </row>
     <row r="1431" spans="1:21" s="20" customFormat="1">
       <c r="A1431" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1431" s="5">
         <v>34714.453200000004</v>
@@ -54354,7 +54354,7 @@
     </row>
     <row r="1432" spans="1:21" s="20" customFormat="1">
       <c r="A1432" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1432" s="5">
         <v>35079.695400000004</v>
@@ -54372,7 +54372,7 @@
     </row>
     <row r="1433" spans="1:21" s="20" customFormat="1">
       <c r="A1433" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1433" s="5">
         <v>35444.937600000005</v>
@@ -54390,7 +54390,7 @@
     </row>
     <row r="1434" spans="1:21" s="20" customFormat="1">
       <c r="A1434" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1434" s="5">
         <v>35810.179800000005</v>
@@ -54408,7 +54408,7 @@
     </row>
     <row r="1435" spans="1:21" s="20" customFormat="1">
       <c r="A1435" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1435" s="5">
         <v>36175.422000000006</v>
@@ -54426,7 +54426,7 @@
     </row>
     <row r="1436" spans="1:21" s="20" customFormat="1">
       <c r="A1436" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1436" s="5">
         <v>36540.664200000007</v>
@@ -54444,7 +54444,7 @@
     </row>
     <row r="1437" spans="1:21" s="20" customFormat="1">
       <c r="A1437" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1437" s="5">
         <v>36905.906400000007</v>
@@ -54462,7 +54462,7 @@
     </row>
     <row r="1438" spans="1:21" s="20" customFormat="1">
       <c r="A1438" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B1438" s="5">
         <v>37271.148600000008</v>
@@ -54480,7 +54480,7 @@
     </row>
     <row r="1439" spans="1:21" s="20" customFormat="1">
       <c r="A1439" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B1439" s="5">
         <v>24303</v>
@@ -54499,7 +54499,7 @@
     </row>
     <row r="1440" spans="1:21" s="20" customFormat="1">
       <c r="A1440" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B1440" s="5">
         <f>B$1439+365.25*C1440</f>
@@ -54520,7 +54520,7 @@
     </row>
     <row r="1441" spans="1:36" s="20" customFormat="1">
       <c r="A1441" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B1441" s="5">
         <f>B$1439+365.25*C1441</f>
@@ -54571,7 +54571,7 @@
     </row>
     <row r="1442" spans="1:36">
       <c r="A1442" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1442" s="5">
         <v>35200</v>
@@ -54594,7 +54594,7 @@
     </row>
     <row r="1443" spans="1:36">
       <c r="A1443" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1443" s="5">
         <f>B$1442+365.25*C1443</f>
@@ -54618,7 +54618,7 @@
     </row>
     <row r="1444" spans="1:36">
       <c r="A1444" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1444" s="5">
         <f t="shared" ref="B1444:B1449" si="18">B$1442+365.25*C1444</f>
@@ -54647,7 +54647,7 @@
     </row>
     <row r="1445" spans="1:36">
       <c r="A1445" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1445" s="5">
         <f t="shared" ref="B1445" si="19">B$1442+365.25*C1445</f>
@@ -54693,7 +54693,7 @@
     </row>
     <row r="1446" spans="1:36">
       <c r="A1446" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1446" s="5">
         <f t="shared" si="18"/>
@@ -54747,7 +54747,7 @@
     </row>
     <row r="1447" spans="1:36">
       <c r="A1447" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1447" s="5">
         <f t="shared" si="18"/>
@@ -54778,7 +54778,7 @@
     </row>
     <row r="1448" spans="1:36">
       <c r="A1448" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1448" s="5">
         <f t="shared" si="18"/>
@@ -54809,7 +54809,7 @@
     </row>
     <row r="1449" spans="1:36">
       <c r="A1449" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B1449" s="5">
         <f t="shared" si="18"/>
@@ -54842,7 +54842,7 @@
     </row>
     <row r="1450" spans="1:36">
       <c r="A1450" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B1450" s="54">
         <v>36600</v>
@@ -54859,7 +54859,7 @@
     </row>
     <row r="1451" spans="1:36">
       <c r="A1451" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B1451" s="5">
         <f>B$1450+365.25*C1451</f>
@@ -54890,7 +54890,7 @@
     </row>
     <row r="1452" spans="1:36">
       <c r="A1452" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B1452" s="5">
         <f t="shared" ref="B1452:B1455" si="20">B$1450+365.25*C1452</f>
@@ -54921,7 +54921,7 @@
     </row>
     <row r="1453" spans="1:36">
       <c r="A1453" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B1453" s="5">
         <f t="shared" si="20"/>
@@ -54954,7 +54954,7 @@
     </row>
     <row r="1454" spans="1:36">
       <c r="A1454" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B1454" s="5">
         <f t="shared" si="20"/>
@@ -54975,7 +54975,7 @@
     </row>
     <row r="1455" spans="1:36">
       <c r="A1455" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B1455" s="5">
         <f t="shared" si="20"/>
@@ -55001,7 +55001,7 @@
     </row>
     <row r="1456" spans="1:36">
       <c r="A1456" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B1456" s="54">
         <v>37408</v>
@@ -55018,7 +55018,7 @@
     </row>
     <row r="1457" spans="1:32">
       <c r="A1457" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B1457" s="54">
         <f>B$1456+365.25*C1457</f>
@@ -55043,7 +55043,7 @@
     </row>
     <row r="1458" spans="1:32">
       <c r="A1458" s="56" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1458" s="5">
         <v>36285</v>
@@ -55060,7 +55060,7 @@
     </row>
     <row r="1459" spans="1:32">
       <c r="A1459" s="56" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1459" s="54">
         <f>B$1458+365.25*C1459</f>
@@ -55083,7 +55083,7 @@
     </row>
     <row r="1460" spans="1:32">
       <c r="A1460" s="56" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1460" s="54">
         <f t="shared" ref="B1460" si="21">B$1458+365.25*C1460</f>
@@ -55115,7 +55115,7 @@
     </row>
     <row r="1461" spans="1:32">
       <c r="A1461" s="56" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1461" s="54">
         <f>B$1458+365.25*C1461</f>
@@ -55147,7 +55147,7 @@
     </row>
     <row r="1462" spans="1:32">
       <c r="A1462" s="56" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1462" s="54">
         <f>B$1458+365.25*C1462</f>
@@ -55167,7 +55167,7 @@
     </row>
     <row r="1463" spans="1:32">
       <c r="A1463" s="56" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1463" s="54">
         <f>B$1458+365.25*C1463</f>
@@ -55199,7 +55199,7 @@
     </row>
     <row r="1464" spans="1:32">
       <c r="A1464" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1464" s="54">
         <v>13346</v>
@@ -55216,7 +55216,7 @@
     </row>
     <row r="1465" spans="1:32">
       <c r="A1465" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1465" s="54">
         <f>B$1464+365.25*C1465</f>
@@ -55241,7 +55241,7 @@
     </row>
     <row r="1466" spans="1:32">
       <c r="A1466" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1466" s="54">
         <f t="shared" ref="B1466:B1481" si="23">B$1464+365.25*C1466</f>
@@ -55266,7 +55266,7 @@
     </row>
     <row r="1467" spans="1:32">
       <c r="A1467" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1467" s="54">
         <f t="shared" si="23"/>
@@ -55291,7 +55291,7 @@
     </row>
     <row r="1468" spans="1:32">
       <c r="A1468" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1468" s="54">
         <f t="shared" si="23"/>
@@ -55316,7 +55316,7 @@
     </row>
     <row r="1469" spans="1:32">
       <c r="A1469" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1469" s="54">
         <f t="shared" si="23"/>
@@ -55341,7 +55341,7 @@
     </row>
     <row r="1470" spans="1:32">
       <c r="A1470" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1470" s="54">
         <f t="shared" si="23"/>
@@ -55366,7 +55366,7 @@
     </row>
     <row r="1471" spans="1:32">
       <c r="A1471" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1471" s="54">
         <f t="shared" si="23"/>
@@ -55389,7 +55389,7 @@
     </row>
     <row r="1472" spans="1:32">
       <c r="A1472" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1472" s="54">
         <f t="shared" si="23"/>
@@ -55414,7 +55414,7 @@
     </row>
     <row r="1473" spans="1:30">
       <c r="A1473" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1473" s="54">
         <f t="shared" si="23"/>
@@ -55437,7 +55437,7 @@
     </row>
     <row r="1474" spans="1:30">
       <c r="A1474" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1474" s="54">
         <f t="shared" si="23"/>
@@ -55460,7 +55460,7 @@
     </row>
     <row r="1475" spans="1:30">
       <c r="A1475" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1475" s="54">
         <f t="shared" si="23"/>
@@ -55485,7 +55485,7 @@
     </row>
     <row r="1476" spans="1:30">
       <c r="A1476" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1476" s="54">
         <f t="shared" si="23"/>
@@ -55508,7 +55508,7 @@
     </row>
     <row r="1477" spans="1:30">
       <c r="A1477" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1477" s="54">
         <f t="shared" si="23"/>
@@ -55533,7 +55533,7 @@
     </row>
     <row r="1478" spans="1:30">
       <c r="A1478" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1478" s="54">
         <f t="shared" si="23"/>
@@ -55556,7 +55556,7 @@
     </row>
     <row r="1479" spans="1:30">
       <c r="A1479" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1479" s="54">
         <f t="shared" si="23"/>
@@ -55579,7 +55579,7 @@
     </row>
     <row r="1480" spans="1:30">
       <c r="A1480" s="56" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B1480" s="54">
         <f t="shared" si="23"/>
@@ -55604,7 +55604,7 @@
     </row>
     <row r="1481" spans="1:30">
       <c r="A1481" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1481" s="54">
         <f t="shared" si="23"/>
@@ -55622,7 +55622,7 @@
     </row>
     <row r="1482" spans="1:30">
       <c r="A1482" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1482" s="54">
         <f>B$1481+365.25*C1482</f>
@@ -55647,7 +55647,7 @@
     </row>
     <row r="1483" spans="1:30">
       <c r="A1483" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1483" s="54">
         <f t="shared" ref="B1483:B1505" si="25">B$1481+365.25*C1483</f>
@@ -55672,7 +55672,7 @@
     </row>
     <row r="1484" spans="1:30">
       <c r="A1484" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1484" s="54">
         <f t="shared" si="25"/>
@@ -55697,7 +55697,7 @@
     </row>
     <row r="1485" spans="1:30">
       <c r="A1485" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1485" s="54">
         <f t="shared" si="25"/>
@@ -55722,7 +55722,7 @@
     </row>
     <row r="1486" spans="1:30">
       <c r="A1486" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1486" s="54">
         <f t="shared" si="25"/>
@@ -55747,7 +55747,7 @@
     </row>
     <row r="1487" spans="1:30">
       <c r="A1487" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1487" s="54">
         <f t="shared" si="25"/>
@@ -55770,7 +55770,7 @@
     </row>
     <row r="1488" spans="1:30">
       <c r="A1488" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1488" s="54">
         <f t="shared" si="25"/>
@@ -55795,7 +55795,7 @@
     </row>
     <row r="1489" spans="1:30">
       <c r="A1489" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1489" s="54">
         <f t="shared" si="25"/>
@@ -55818,7 +55818,7 @@
     </row>
     <row r="1490" spans="1:30">
       <c r="A1490" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1490" s="54">
         <f t="shared" si="25"/>
@@ -55841,7 +55841,7 @@
     </row>
     <row r="1491" spans="1:30">
       <c r="A1491" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1491" s="54">
         <f t="shared" si="25"/>
@@ -55866,7 +55866,7 @@
     </row>
     <row r="1492" spans="1:30">
       <c r="A1492" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1492" s="54">
         <f t="shared" si="25"/>
@@ -55889,7 +55889,7 @@
     </row>
     <row r="1493" spans="1:30">
       <c r="A1493" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1493" s="54">
         <f t="shared" si="25"/>
@@ -55912,7 +55912,7 @@
     </row>
     <row r="1494" spans="1:30">
       <c r="A1494" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1494" s="54">
         <f t="shared" si="25"/>
@@ -55937,7 +55937,7 @@
     </row>
     <row r="1495" spans="1:30">
       <c r="A1495" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1495" s="54">
         <f t="shared" si="25"/>
@@ -55962,7 +55962,7 @@
     </row>
     <row r="1496" spans="1:30">
       <c r="A1496" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1496" s="54">
         <f t="shared" si="25"/>
@@ -55987,7 +55987,7 @@
     </row>
     <row r="1497" spans="1:30">
       <c r="A1497" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1497" s="54">
         <f t="shared" si="25"/>
@@ -56010,7 +56010,7 @@
     </row>
     <row r="1498" spans="1:30">
       <c r="A1498" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1498" s="54">
         <f t="shared" si="25"/>
@@ -56035,7 +56035,7 @@
     </row>
     <row r="1499" spans="1:30">
       <c r="A1499" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1499" s="54">
         <f t="shared" si="25"/>
@@ -56060,7 +56060,7 @@
     </row>
     <row r="1500" spans="1:30">
       <c r="A1500" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1500" s="54">
         <f t="shared" si="25"/>
@@ -56083,7 +56083,7 @@
     </row>
     <row r="1501" spans="1:30">
       <c r="A1501" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1501" s="54">
         <f t="shared" si="25"/>
@@ -56106,7 +56106,7 @@
     </row>
     <row r="1502" spans="1:30">
       <c r="A1502" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1502" s="54">
         <f t="shared" si="25"/>
@@ -56129,7 +56129,7 @@
     </row>
     <row r="1503" spans="1:30">
       <c r="A1503" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1503" s="54">
         <f t="shared" si="25"/>
@@ -56154,7 +56154,7 @@
     </row>
     <row r="1504" spans="1:30">
       <c r="A1504" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1504" s="54">
         <f t="shared" si="25"/>
@@ -56177,7 +56177,7 @@
     </row>
     <row r="1505" spans="1:30">
       <c r="A1505" s="56" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B1505" s="54">
         <f t="shared" si="25"/>

</xml_diff>